<commit_message>
Update to high-risk group timeseries script
</commit_message>
<xml_diff>
--- a/data/input/static/metadata_timeseries_country_month.xlsx
+++ b/data/input/static/metadata_timeseries_country_month.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://worldhealthorg.sharepoint.com/sites/COVID19VaccineDeliveryFacility-DataAnalyticsandMonitoring/Shared Documents/Data, Analytics, and Monitoring/02 Analysis/01 Static datasets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="97" documentId="8_{CCFBF1C8-C3FD-4E70-8738-04DDFC841C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{01115255-4A6F-4059-A97F-81CFC3C416A9}"/>
+  <xr:revisionPtr revIDLastSave="242" documentId="8_{CCFBF1C8-C3FD-4E70-8738-04DDFC841C33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B4029C3C-A873-478B-8942-CF0B96CD691A}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="14400" windowHeight="7360" xr2:uid="{B7668904-28FE-4CEA-A556-9FF33A6F2EDC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{B7668904-28FE-4CEA-A556-9FF33A6F2EDC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="259" uniqueCount="102">
   <si>
     <t>indicator</t>
   </si>
@@ -193,6 +193,153 @@
   </si>
   <si>
     <t>WHO COVmart; UNICEF MDB</t>
+  </si>
+  <si>
+    <t>adm_a1d_add</t>
+  </si>
+  <si>
+    <t>adm_a1d_month</t>
+  </si>
+  <si>
+    <t>adm_fv_add</t>
+  </si>
+  <si>
+    <t>adm_fv_month</t>
+  </si>
+  <si>
+    <t>adm_booster_add</t>
+  </si>
+  <si>
+    <t>adm_booster_month</t>
+  </si>
+  <si>
+    <t>cov_total_a1d</t>
+  </si>
+  <si>
+    <t>cov_total_booster</t>
+  </si>
+  <si>
+    <t>cov_total_fv</t>
+  </si>
+  <si>
+    <t>adm_hcw_a1d_add</t>
+  </si>
+  <si>
+    <t>adm_hcw_fv_add</t>
+  </si>
+  <si>
+    <t>adm_hcw_booster_add</t>
+  </si>
+  <si>
+    <t>cov_hcw_fv</t>
+  </si>
+  <si>
+    <t>cov_hcw_booster</t>
+  </si>
+  <si>
+    <t>cov_hcw_a1d</t>
+  </si>
+  <si>
+    <t>adm_old_a1d_add</t>
+  </si>
+  <si>
+    <t>adm_old_fv_add</t>
+  </si>
+  <si>
+    <t>adm_old_booster_add</t>
+  </si>
+  <si>
+    <t>cov_old_a1d</t>
+  </si>
+  <si>
+    <t>cov_old_fv</t>
+  </si>
+  <si>
+    <t>cov_old_booster</t>
+  </si>
+  <si>
+    <t>Percentage</t>
+  </si>
+  <si>
+    <t>WHO WIISEmart</t>
+  </si>
+  <si>
+    <t>pop_hcw</t>
+  </si>
+  <si>
+    <t>pop_older</t>
+  </si>
+  <si>
+    <t>Population, total healthcare workers</t>
+  </si>
+  <si>
+    <t>Population, older adults (as defined by country)</t>
+  </si>
+  <si>
+    <t>ILO Stat</t>
+  </si>
+  <si>
+    <t>Individuals having received at least one dose, cumulative</t>
+  </si>
+  <si>
+    <t>Individuals having received at least one dose, net during the month indicated</t>
+  </si>
+  <si>
+    <t>Individuals having received a complete primary series, cumulative</t>
+  </si>
+  <si>
+    <t>Individuals having received a complete primary series, net during the month indicated</t>
+  </si>
+  <si>
+    <t>Individuals having received a first booster, cumulative</t>
+  </si>
+  <si>
+    <t>Individuals having received a first booster, net during the month indicated</t>
+  </si>
+  <si>
+    <t>Individuals with at least one dose, as percentage of total population</t>
+  </si>
+  <si>
+    <t>Individuals with a complete primary series, as percentage of total population</t>
+  </si>
+  <si>
+    <t>Individuals having received a booster / additional dose, as percentage of total population</t>
+  </si>
+  <si>
+    <t>Healthcare workers with at least one dose, as percentage of total healthcare worker population</t>
+  </si>
+  <si>
+    <t>Healthcare workers with a complete primary series (adjusted), as percentage of total healthcare worker population</t>
+  </si>
+  <si>
+    <t>Older adults with at least one dose, as percentage of older adult population</t>
+  </si>
+  <si>
+    <t>Older adults with a complete primary series, as percentage of older adult population</t>
+  </si>
+  <si>
+    <t>Older adults with a first booster dose, as percentage of older adult population</t>
+  </si>
+  <si>
+    <t>Healthcare workers with a first booster dose, as percentage of total healthcare worker population</t>
+  </si>
+  <si>
+    <t>Healthcare workers having received at least one dose, cumulative</t>
+  </si>
+  <si>
+    <t>Healthcare workers having received a complete primary series, cumulative</t>
+  </si>
+  <si>
+    <t>Healthcare workers having received a first booster dose, cumulative</t>
+  </si>
+  <si>
+    <t>Older adults having received at least one dose, cumulative</t>
+  </si>
+  <si>
+    <t>Older adults having received a complete primary series, cumulative</t>
+  </si>
+  <si>
+    <t>Older adults having received a first booster dose, cumulative</t>
   </si>
 </sst>
 </file>
@@ -248,8 +395,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ED3BA5C5-A422-4B35-AD44-580AA5D25570}" name="Table3" displayName="Table3" ref="A1:G14" totalsRowShown="0">
-  <autoFilter ref="A1:G14" xr:uid="{ED3BA5C5-A422-4B35-AD44-580AA5D25570}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{ED3BA5C5-A422-4B35-AD44-580AA5D25570}" name="Table3" displayName="Table3" ref="A1:G37" totalsRowShown="0">
+  <autoFilter ref="A1:G37" xr:uid="{ED3BA5C5-A422-4B35-AD44-580AA5D25570}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{07102CF5-A931-4583-85B2-728843922D11}" name="indicator"/>
     <tableColumn id="2" xr3:uid="{B4182467-F853-48FA-BEDF-1162616E9E0F}" name="description"/>
@@ -560,24 +707,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4170C720-B170-49EB-B0F0-5DE9F2B19454}">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="58.54296875" customWidth="1"/>
-    <col min="3" max="3" width="8.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.81640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="25.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="104.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -600,7 +745,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>37</v>
       </c>
@@ -623,7 +768,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>27</v>
       </c>
@@ -646,7 +791,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>34</v>
       </c>
@@ -669,7 +814,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>24</v>
       </c>
@@ -692,7 +837,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>20</v>
       </c>
@@ -715,7 +860,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>38</v>
       </c>
@@ -738,7 +883,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -761,35 +906,35 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>76</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>78</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="D9" t="s">
         <v>8</v>
       </c>
       <c r="E9" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
       <c r="F9" t="s">
-        <v>17</v>
+        <v>80</v>
       </c>
       <c r="G9" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>77</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>79</v>
       </c>
       <c r="C10" t="s">
         <v>7</v>
@@ -798,44 +943,44 @@
         <v>8</v>
       </c>
       <c r="E10" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F10" t="s">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="G10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C11" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="D11" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="F11" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="G11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C12" t="s">
         <v>7</v>
@@ -847,18 +992,18 @@
         <v>12</v>
       </c>
       <c r="F12" t="s">
-        <v>23</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C13" t="s">
         <v>7</v>
@@ -870,32 +1015,561 @@
         <v>12</v>
       </c>
       <c r="F13" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>53</v>
+      </c>
+      <c r="B14" t="s">
+        <v>81</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" t="s">
+        <v>8</v>
+      </c>
+      <c r="E14" t="s">
+        <v>9</v>
+      </c>
+      <c r="F14" t="s">
+        <v>10</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>54</v>
+      </c>
+      <c r="B15" t="s">
+        <v>82</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" t="s">
+        <v>9</v>
+      </c>
+      <c r="F15" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>55</v>
+      </c>
+      <c r="B16" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" t="s">
+        <v>9</v>
+      </c>
+      <c r="F16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>56</v>
+      </c>
+      <c r="B17" t="s">
+        <v>84</v>
+      </c>
+      <c r="C17" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" t="s">
+        <v>9</v>
+      </c>
+      <c r="F17" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18" t="s">
+        <v>85</v>
+      </c>
+      <c r="C18" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18" t="s">
+        <v>8</v>
+      </c>
+      <c r="E18" t="s">
+        <v>9</v>
+      </c>
+      <c r="F18" t="s">
+        <v>10</v>
+      </c>
+      <c r="G18" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" t="s">
+        <v>86</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F19" t="s">
+        <v>10</v>
+      </c>
+      <c r="G19" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>59</v>
+      </c>
+      <c r="B20" t="s">
+        <v>87</v>
+      </c>
+      <c r="C20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" t="s">
+        <v>74</v>
+      </c>
+      <c r="F20" t="s">
+        <v>10</v>
+      </c>
+      <c r="G20" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+      <c r="C21" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" t="s">
+        <v>74</v>
+      </c>
+      <c r="F21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>60</v>
+      </c>
+      <c r="B22" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
+      </c>
+      <c r="F22" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" t="s">
+        <v>96</v>
+      </c>
+      <c r="C23" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" t="s">
+        <v>9</v>
+      </c>
+      <c r="F23" t="s">
+        <v>75</v>
+      </c>
+      <c r="G23" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>63</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
+        <v>7</v>
+      </c>
+      <c r="D24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" t="s">
+        <v>9</v>
+      </c>
+      <c r="F24" t="s">
+        <v>75</v>
+      </c>
+      <c r="G24" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>64</v>
+      </c>
+      <c r="B25" t="s">
+        <v>98</v>
+      </c>
+      <c r="C25" t="s">
+        <v>7</v>
+      </c>
+      <c r="D25" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" t="s">
+        <v>9</v>
+      </c>
+      <c r="F25" t="s">
+        <v>75</v>
+      </c>
+      <c r="G25" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>67</v>
+      </c>
+      <c r="B26" t="s">
+        <v>90</v>
+      </c>
+      <c r="C26" t="s">
+        <v>7</v>
+      </c>
+      <c r="D26" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" t="s">
+        <v>75</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>65</v>
+      </c>
+      <c r="B27" t="s">
+        <v>91</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" t="s">
+        <v>75</v>
+      </c>
+      <c r="G27" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>66</v>
+      </c>
+      <c r="B28" t="s">
+        <v>95</v>
+      </c>
+      <c r="C28" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" t="s">
+        <v>75</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>68</v>
+      </c>
+      <c r="B29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s">
+        <v>7</v>
+      </c>
+      <c r="D29" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" t="s">
+        <v>9</v>
+      </c>
+      <c r="F29" t="s">
+        <v>75</v>
+      </c>
+      <c r="G29" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>69</v>
+      </c>
+      <c r="B30" t="s">
+        <v>100</v>
+      </c>
+      <c r="C30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" t="s">
+        <v>9</v>
+      </c>
+      <c r="F30" t="s">
+        <v>75</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>70</v>
+      </c>
+      <c r="B31" t="s">
+        <v>101</v>
+      </c>
+      <c r="C31" t="s">
+        <v>7</v>
+      </c>
+      <c r="D31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" t="s">
+        <v>9</v>
+      </c>
+      <c r="F31" t="s">
+        <v>75</v>
+      </c>
+      <c r="G31" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>71</v>
+      </c>
+      <c r="B32" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" t="s">
+        <v>7</v>
+      </c>
+      <c r="D32" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" t="s">
+        <v>74</v>
+      </c>
+      <c r="F32" t="s">
+        <v>75</v>
+      </c>
+      <c r="G32" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" t="s">
+        <v>7</v>
+      </c>
+      <c r="D33" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" t="s">
+        <v>74</v>
+      </c>
+      <c r="F33" t="s">
+        <v>75</v>
+      </c>
+      <c r="G33" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>73</v>
+      </c>
+      <c r="B34" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" t="s">
+        <v>7</v>
+      </c>
+      <c r="D34" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" t="s">
+        <v>74</v>
+      </c>
+      <c r="F34" t="s">
+        <v>75</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" t="s">
+        <v>7</v>
+      </c>
+      <c r="D35" t="s">
+        <v>8</v>
+      </c>
+      <c r="E35" t="s">
+        <v>12</v>
+      </c>
+      <c r="F35" t="s">
         <v>23</v>
       </c>
-      <c r="G13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" t="s">
+        <v>12</v>
+      </c>
+      <c r="F36" t="s">
+        <v>23</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>44</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B37" t="s">
         <v>50</v>
       </c>
-      <c r="C14" t="s">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>14</v>
-      </c>
-      <c r="E14" t="s">
+      <c r="C37" t="s">
+        <v>7</v>
+      </c>
+      <c r="D37" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" t="s">
         <v>12</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F37" t="s">
         <v>52</v>
       </c>
-      <c r="G14" t="s">
+      <c r="G37" t="s">
         <v>11</v>
       </c>
     </row>
@@ -908,6 +1582,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001F87334A6AC30D4EA6021977FA7E2445" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="13eff9136b4917bb459ad9c1db870f6d">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="b370a6fa-a798-42e0-969d-19c284d8683f" xmlns:ns3="62ca1376-8bea-4949-825e-fec085c3924e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="60e7197df19c7150b1ba0c3bfe00adf4" ns2:_="" ns3:_="">
     <xsd:import namespace="b370a6fa-a798-42e0-969d-19c284d8683f"/>
@@ -1124,15 +1807,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -1140,6 +1814,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4627CB4-3356-4239-9CEE-5D697A543E8C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8D0F9EFB-FA02-4183-BFA5-CB4679DC86A9}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1158,14 +1840,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F4627CB4-3356-4239-9CEE-5D697A543E8C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9666D219-5436-480B-874A-B0985F4B1352}">
   <ds:schemaRefs>

</xml_diff>